<commit_message>
export remaining quote functions to excel (694/1114)
</commit_message>
<xml_diff>
--- a/UnitTests/Tests/Quotes.xlsx
+++ b/UnitTests/Tests/Quotes.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
   <si>
     <t>Function</t>
   </si>
@@ -112,33 +112,6 @@
   </si>
   <si>
     <t>qlRelinkableHandleQuote</t>
-  </si>
-  <si>
-    <t>quote01#0000</t>
-  </si>
-  <si>
-    <t>quote02#0000</t>
-  </si>
-  <si>
-    <t>quote03#0000</t>
-  </si>
-  <si>
-    <t>quote04#0000</t>
-  </si>
-  <si>
-    <t>quote05#0000</t>
-  </si>
-  <si>
-    <t>quote06#0000</t>
-  </si>
-  <si>
-    <t>quote07#0000</t>
-  </si>
-  <si>
-    <t>quote08#0000</t>
-  </si>
-  <si>
-    <t>quote09#0000</t>
   </si>
 </sst>
 </file>
@@ -554,7 +527,7 @@
         <v>FAIL</v>
       </c>
       <c r="E3">
-        <f>_xll.qlQuoteValue(E12)</f>
+        <f>_xll.qlQuoteValue(F12)</f>
         <v>123</v>
       </c>
     </row>
@@ -570,7 +543,7 @@
         <v>FAIL</v>
       </c>
       <c r="E4" t="b">
-        <f>_xll.qlQuoteIsValid(E12)</f>
+        <f>_xll.qlQuoteIsValid(F12)</f>
         <v>1</v>
       </c>
     </row>
@@ -591,7 +564,7 @@
       </c>
       <c r="F5" t="str">
         <f>_xll.qlSimpleQuote(,123)</f>
-        <v>obj_0008b#0000</v>
+        <v>obj_00009#0002</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -611,7 +584,7 @@
       </c>
       <c r="F6" t="str">
         <f>_xll.qlSimpleQuote(,123)</f>
-        <v>obj_00083#0000</v>
+        <v>obj_00008#0002</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -631,7 +604,7 @@
       </c>
       <c r="F7" t="str">
         <f>_xll.qlSimpleQuote(,123)</f>
-        <v>obj_00090#0000</v>
+        <v>obj_00007#0002</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -646,7 +619,7 @@
         <v>FAIL</v>
       </c>
       <c r="E8">
-        <f>_xll.qlSimpleQuoteTickValue(E12)</f>
+        <f>_xll.qlSimpleQuoteTickValue(F12)</f>
         <v>456</v>
       </c>
     </row>
@@ -681,36 +654,44 @@
       <c r="A12" t="s">
         <v>17</v>
       </c>
-      <c r="B12" t="s">
-        <v>31</v>
+      <c r="B12" t="b">
+        <v>0</v>
       </c>
       <c r="D12" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>FAIL</v>
-      </c>
-      <c r="E12" t="str">
-        <f>_xll.qlSimpleQuote("quote01",123,456)</f>
-        <v>quote01#0000</v>
+        <v>PASS</v>
+      </c>
+      <c r="E12" t="b">
+        <f>ISERROR(F12)</f>
+        <v>0</v>
+      </c>
+      <c r="F12" t="str">
+        <f>_xll.qlSimpleQuote(,123,456)</f>
+        <v>obj_00003#0003</v>
       </c>
       <c r="H12" t="str">
         <f>_xll.qlIborIndex(,"euribor","1y",2,"eur","target","Modified Following",TRUE,"Actual/360")</f>
-        <v>obj_00084#0000</v>
+        <v>obj_00000#0002</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>18</v>
       </c>
-      <c r="B13" t="s">
-        <v>32</v>
+      <c r="B13" t="b">
+        <v>0</v>
       </c>
       <c r="D13" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>FAIL</v>
-      </c>
-      <c r="E13" t="str">
-        <f>_xll.qlForwardValueQuote("quote02",H12,H13)</f>
-        <v>quote02#0000</v>
+        <v>PASS</v>
+      </c>
+      <c r="E13" t="b">
+        <f t="shared" ref="E13:E18" si="1">ISERROR(F13)</f>
+        <v>0</v>
+      </c>
+      <c r="F13" t="str">
+        <f>_xll.qlForwardValueQuote(,H12,H13)</f>
+        <v>obj_0000d#0003</v>
       </c>
       <c r="H13" s="4">
         <v>25569</v>
@@ -720,87 +701,107 @@
       <c r="A14" t="s">
         <v>19</v>
       </c>
-      <c r="B14" t="s">
-        <v>33</v>
+      <c r="B14" t="b">
+        <v>0</v>
       </c>
       <c r="D14" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>FAIL</v>
-      </c>
-      <c r="E14" t="str">
-        <f>_xll.qlForwardSwapQuote("quote03",H14,123,"1y")</f>
-        <v>quote03#0000</v>
+        <v>PASS</v>
+      </c>
+      <c r="E14" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F14" t="str">
+        <f>_xll.qlForwardSwapQuote(,H14,123,"1y")</f>
+        <v>obj_0000c#0003</v>
       </c>
       <c r="H14" t="str">
         <f>_xll.qlSwapIndex(,"euribor","1y",2,"eur","target","1y","Modified Following","Actual/360",H12)</f>
-        <v>obj_00088#0000</v>
+        <v>obj_0000a#0002</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>20</v>
       </c>
-      <c r="B15" t="s">
-        <v>34</v>
+      <c r="B15" t="b">
+        <v>0</v>
       </c>
       <c r="D15" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>FAIL</v>
-      </c>
-      <c r="E15" t="str">
-        <f>_xll.qlImpliedStdDevQuote("quote04","Call",123,456,789)</f>
-        <v>quote04#0000</v>
+        <v>PASS</v>
+      </c>
+      <c r="E15" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F15" t="str">
+        <f>_xll.qlImpliedStdDevQuote(,"Call",123,456,789)</f>
+        <v>obj_00004#0003</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>21</v>
       </c>
-      <c r="B16" t="s">
-        <v>35</v>
+      <c r="B16" t="b">
+        <v>0</v>
       </c>
       <c r="D16" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>FAIL</v>
-      </c>
-      <c r="E16" t="str">
-        <f>_xll.qlEurodollarFuturesImpliedStdDevQuote("quote05",123,456,F6,123)</f>
-        <v>quote05#0000</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>PASS</v>
+      </c>
+      <c r="E16" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F16" t="str">
+        <f>_xll.qlEurodollarFuturesImpliedStdDevQuote(,123,456,F6,123)</f>
+        <v>obj_0000b#0003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>22</v>
       </c>
-      <c r="B17" t="s">
-        <v>36</v>
+      <c r="B17" t="b">
+        <v>0</v>
       </c>
       <c r="D17" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>FAIL</v>
-      </c>
-      <c r="E17" t="str">
-        <f>_xll.qlCompositeQuote("quote06",1,2,"+")</f>
-        <v>quote06#0000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>PASS</v>
+      </c>
+      <c r="E17" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F17" t="str">
+        <f>_xll.qlCompositeQuote(,1,2,"+")</f>
+        <v>obj_00002#0003</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>23</v>
       </c>
-      <c r="B18" t="s">
-        <v>37</v>
+      <c r="B18" t="b">
+        <v>0</v>
       </c>
       <c r="D18" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>FAIL</v>
-      </c>
-      <c r="E18" t="str">
-        <f>_xll.qlFuturesConvAdjustmentQuote("quote07",H12,"H9",123,456,789)</f>
-        <v>quote07#0000</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>PASS</v>
+      </c>
+      <c r="E18" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F18" t="str">
+        <f>_xll.qlFuturesConvAdjustmentQuote(,H12,"H9",123,456,789)</f>
+        <v>obj_00006#0003</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -812,11 +813,11 @@
         <v>FAIL</v>
       </c>
       <c r="E19">
-        <f>_xll.qlFuturesConvAdjustmentQuoteVolatility(E18)</f>
+        <f>_xll.qlFuturesConvAdjustmentQuoteVolatility(F18)</f>
         <v>456</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -828,11 +829,11 @@
         <v>FAIL</v>
       </c>
       <c r="E20">
-        <f>_xll.qlFuturesConvAdjustmentQuoteMeanReversion(E18)</f>
+        <f>_xll.qlFuturesConvAdjustmentQuoteMeanReversion(F18)</f>
         <v>789</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -844,11 +845,11 @@
         <v>FAIL</v>
       </c>
       <c r="E21">
-        <f>_xll.qlFuturesConvAdjustmentQuoteImmDate(E18)</f>
+        <f>_xll.qlFuturesConvAdjustmentQuoteImmDate(F18)</f>
         <v>43544</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -860,56 +861,64 @@
         <v>FAIL</v>
       </c>
       <c r="E22">
-        <f>_xll.qlFuturesConvAdjustmentQuoteFuturesValue(E18)</f>
+        <f>_xll.qlFuturesConvAdjustmentQuoteFuturesValue(F18)</f>
         <v>123</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>28</v>
       </c>
-      <c r="B23" t="s">
-        <v>38</v>
+      <c r="B23" t="b">
+        <v>0</v>
       </c>
       <c r="D23" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>FAIL</v>
-      </c>
-      <c r="E23" t="str">
-        <f>_xll.qlLastFixingQuote("quote08",H12)</f>
-        <v>quote08#0000</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>PASS</v>
+      </c>
+      <c r="E23" t="b">
+        <f t="shared" ref="E23" si="2">ISERROR(F23)</f>
+        <v>0</v>
+      </c>
+      <c r="F23" t="str">
+        <f>_xll.qlLastFixingQuote(,H12)</f>
+        <v>obj_00001#0003</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>29</v>
       </c>
-      <c r="B24">
-        <v>42644</v>
+      <c r="B24" t="e">
+        <v>#NUM!</v>
       </c>
       <c r="D24" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>FAIL</v>
-      </c>
-      <c r="E24">
-        <f>_xll.qlLastFixingQuoteReferenceDate(E23)</f>
-        <v>42644</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+        <v>ERROR</v>
+      </c>
+      <c r="E24" t="e">
+        <f>_xll.qlLastFixingQuoteReferenceDate(F23)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>30</v>
       </c>
-      <c r="B25" t="s">
-        <v>39</v>
+      <c r="B25" t="b">
+        <v>0</v>
       </c>
       <c r="D25" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>FAIL</v>
-      </c>
-      <c r="E25" t="str">
-        <f>_xll.qlRelinkableHandleQuote("quote09")</f>
-        <v>quote09#0000</v>
+        <v>PASS</v>
+      </c>
+      <c r="E25" t="b">
+        <f t="shared" ref="E25" si="3">ISERROR(F25)</f>
+        <v>0</v>
+      </c>
+      <c r="F25" t="str">
+        <f>_xll.qlRelinkableHandleQuote()</f>
+        <v>obj_00005#0003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>